<commit_message>
Added seeding into GA and visualisation script for plotting and outputting shp files of results
</commit_message>
<xml_diff>
--- a/Optimisation_Cost_Basis.xlsx
+++ b/Optimisation_Cost_Basis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\AU\Melbourne\Service\Water Infrastructure\01 - Business Group\07 - Strategic Intiatives\02 - Future of Water\01 - Retrospective Optimisation of the Tongala WDN\02 - WIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ghdnet-my.sharepoint.com/personal/david_le_ghd_com/Documents/Desktop/WDNOptimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC97D58-054A-415C-96C3-5E900D7ADA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{FCC97D58-054A-415C-96C3-5E900D7ADA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1AB3501-937F-4739-9F8A-60AF2DFB73B0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-420" windowWidth="38640" windowHeight="21390" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pipes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Pumps!$A$1:$E$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Pumps!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -135,13 +135,19 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -163,6 +169,11 @@
       <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3794FF"/>
+      <name val="Var(--vscode-repl-font-family)"/>
     </font>
   </fonts>
   <fills count="6">
@@ -390,18 +401,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -411,36 +424,42 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="6" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="3" fillId="5" borderId="6" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="6" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="6" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="6" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="4" fillId="5" borderId="6" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="6" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="6" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="6" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="5" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="6" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="5" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency 2" xfId="4" xr:uid="{FACBB8EF-27F7-4E29-949F-2F76F0780203}"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{D9958B50-1372-4D89-9565-C28CBD045E04}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,6 +489,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PS4-TDC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -502,99 +546,226 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Pipes!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PS4 - TDC $/m</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
-              <c:f>Pipes!$A$2:$A$8</c:f>
+              <c:f>Pipes!$A$2:$A$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>225</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="15">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="17">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="18">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="19">
                   <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Pipes!$B$2:$B$8</c:f>
+              <c:f>Pipes!$B$2:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>239</c:v>
+                  <c:v>362.58707029616613</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>286</c:v>
+                  <c:v>362.58707029616613</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>360</c:v>
+                  <c:v>362.58707029616613</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>455</c:v>
+                  <c:v>362.58707029616613</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>669</c:v>
+                  <c:v>362.58707029616613</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>722</c:v>
+                  <c:v>362.58707029616613</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>915</c:v>
+                  <c:v>362.58707029616613</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>362.58707029616613</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>433.89080378537034</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>433.89080378537034</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>433.89080378537034</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>433.89080378537034</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>546.15625651305356</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>546.15625651305356</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>546.15625651305356</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>546.15625651305356</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>690.28082420399824</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1014.940376686758</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1095.3467144511797</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1326.9359952555494</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1516.4982802920565</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1895.6228503650705</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2021.9977070560751</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2085.1851354015776</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2274.7474204380846</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2653.8719905110988</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2906.6217038931081</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3412.1211306571267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7EFA-4C3D-8DA2-F3219CDBD097}"/>
+              <c16:uniqueId val="{00000000-92CF-4981-B7EA-CDC99FB7C9A5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -606,17 +777,85 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="69464687"/>
-        <c:axId val="69465167"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="69464687"/>
+        <c:axId val="886131712"/>
+        <c:axId val="886128112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="886131712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PS4-TDC</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -626,8 +865,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -654,15 +893,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69465167"/>
+        <c:crossAx val="886128112"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="69465167"/>
+        <c:axId val="886128112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,8 +924,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -713,9 +955,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69464687"/>
+        <c:crossAx val="886131712"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -725,37 +967,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -841,7 +1052,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -868,8 +1079,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -949,11 +1160,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -964,11 +1170,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -980,7 +1181,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1000,9 +1201,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1015,10 +1213,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1058,22 +1256,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1178,8 +1377,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1311,19 +1510,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1337,6 +1537,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1408,42 +1619,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>285756</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>76206</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>76206</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152406</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5ADE951-28A4-ADDD-0F51-BE833E74519C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -1471,7 +1646,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1486,6 +1661,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76ACD4AE-F0E4-EEB6-BFA2-07637893A62A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1904,13 +2115,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
@@ -1925,7 +2136,7 @@
     <col min="15" max="15" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="14.1" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1938,12 +2149,13 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>100</v>
-      </c>
-      <c r="B2" s="13">
-        <v>239</v>
+    <row r="2" spans="1:7">
+      <c r="A2" s="25">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1">
+        <f t="shared" ref="B2:B5" si="0">$B$7</f>
+        <v>362.58707029616613</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -1951,12 +2163,13 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>150</v>
-      </c>
-      <c r="B3" s="13">
-        <v>286</v>
+    <row r="3" spans="1:7">
+      <c r="A3" s="25">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" si="0"/>
+        <v>362.58707029616613</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -1964,12 +2177,13 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>225</v>
-      </c>
-      <c r="B4" s="13">
-        <v>360</v>
+    <row r="4" spans="1:7">
+      <c r="A4" s="25">
+        <v>63</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>362.58707029616613</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -1977,12 +2191,13 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>300</v>
-      </c>
-      <c r="B5" s="13">
-        <v>455</v>
+    <row r="5" spans="1:7">
+      <c r="A5" s="25">
+        <v>75</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>362.58707029616613</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -1990,12 +2205,13 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>375</v>
-      </c>
-      <c r="B6" s="13">
-        <v>669</v>
+    <row r="6" spans="1:7">
+      <c r="A6" s="25">
+        <v>96</v>
+      </c>
+      <c r="B6" s="1">
+        <f>B7</f>
+        <v>362.58707029616613</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -2003,31 +2219,207 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="4">
-        <v>450</v>
+        <v>100</v>
       </c>
       <c r="B7" s="13">
-        <v>722</v>
+        <v>362.58707029616613</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>525</v>
-      </c>
-      <c r="B8" s="13">
-        <v>915</v>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="25">
+        <v>101</v>
+      </c>
+      <c r="B8" s="1">
+        <f>B7</f>
+        <v>362.58707029616613</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="25">
+        <v>103</v>
+      </c>
+      <c r="B9" s="1">
+        <f>B7</f>
+        <v>362.58707029616613</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="25">
+        <v>141</v>
+      </c>
+      <c r="B10" s="1">
+        <f>B12</f>
+        <v>433.89080378537034</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="25">
+        <v>143</v>
+      </c>
+      <c r="B11" s="1">
+        <f>B12</f>
+        <v>433.89080378537034</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="4">
+        <v>150</v>
+      </c>
+      <c r="B12" s="13">
+        <v>433.89080378537034</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="25">
+        <v>158</v>
+      </c>
+      <c r="B13" s="1">
+        <f>B12</f>
+        <v>433.89080378537034</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="25">
+        <v>186</v>
+      </c>
+      <c r="B14" s="1">
+        <f>B16</f>
+        <v>546.15625651305356</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="25">
+        <v>200</v>
+      </c>
+      <c r="B15" s="1">
+        <f>B16</f>
+        <v>546.15625651305356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4">
+        <v>225</v>
+      </c>
+      <c r="B16" s="13">
+        <v>546.15625651305356</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="25">
+        <v>235</v>
+      </c>
+      <c r="B17" s="1">
+        <f>B16</f>
+        <v>546.15625651305356</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4">
+        <v>300</v>
+      </c>
+      <c r="B18" s="13">
+        <v>690.28082420399824</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4">
+        <v>375</v>
+      </c>
+      <c r="B19" s="13">
+        <v>1014.940376686758</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4">
+        <v>450</v>
+      </c>
+      <c r="B20" s="13">
+        <v>1095.3467144511797</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4">
+        <v>525</v>
+      </c>
+      <c r="B21" s="13">
+        <v>1326.9359952555494</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4">
+        <v>600</v>
+      </c>
+      <c r="B22" s="13">
+        <v>1516.4982802920565</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="4">
+        <v>750</v>
+      </c>
+      <c r="B23" s="13">
+        <v>1895.6228503650705</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="4">
+        <v>800</v>
+      </c>
+      <c r="B24" s="13">
+        <v>2021.9977070560751</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="4">
+        <v>825</v>
+      </c>
+      <c r="B25" s="13">
+        <v>2085.1851354015776</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4">
+        <v>900</v>
+      </c>
+      <c r="B26" s="13">
+        <v>2274.7474204380846</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="4">
+        <v>1050</v>
+      </c>
+      <c r="B27" s="13">
+        <v>2653.8719905110988</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="4">
+        <v>1150</v>
+      </c>
+      <c r="B28" s="13">
+        <v>2906.6217038931081</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="4">
+        <v>1350</v>
+      </c>
+      <c r="B29" s="13">
+        <v>3412.1211306571267</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2047,7 +2439,7 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -2055,7 +2447,7 @@
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2063,7 +2455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -2071,7 +2463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="9">
         <v>20</v>
       </c>
@@ -2079,7 +2471,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="9">
         <v>50</v>
       </c>
@@ -2087,7 +2479,7 @@
         <v>1065000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="9">
         <v>100</v>
       </c>
@@ -2095,7 +2487,7 @@
         <v>1230000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="9">
         <v>150</v>
       </c>
@@ -2103,7 +2495,7 @@
         <v>1350000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="9">
         <v>250</v>
       </c>
@@ -2111,7 +2503,7 @@
         <v>1560000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="9">
         <v>500</v>
       </c>
@@ -2119,7 +2511,7 @@
         <v>1920000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="3"/>
     </row>
   </sheetData>
@@ -2137,7 +2529,7 @@
       <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2152,14 +2544,14 @@
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
       <c r="A1" s="17" t="s">
         <v>20</v>
       </c>
@@ -2173,7 +2565,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="21">
         <f>(PI()*8.55422^2)/4*23.24</f>
         <v>1335.6320621513066</v>
@@ -2204,17 +2596,17 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2222,7 +2614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2230,7 +2622,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2238,7 +2630,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2255,21 +2647,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0184009D-9B32-47C3-B5E2-62689D60A945}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2280,7 +2672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2288,7 +2680,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2299,7 +2691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Added pump curve and pump optimisation commented, optimised visualisation plots to improve usage latency
</commit_message>
<xml_diff>
--- a/Optimisation_Cost_Basis.xlsx
+++ b/Optimisation_Cost_Basis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dle\OneDrive - GHD\Desktop\WDNOptimizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ghdnet-my.sharepoint.com/personal/david_le_ghd_com/Documents/Desktop/WDNOptimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE90823-3444-4B27-98FA-B3EAA73B233A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{6AE90823-3444-4B27-98FA-B3EAA73B233A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEB822BB-1136-4DC5-ADF8-B6D909CD4B2C}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-420" windowWidth="38640" windowHeight="21390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pipes" sheetId="1" r:id="rId1"/>
@@ -2120,8 +2120,8 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2595,7 +2595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E6E8E40-7D95-4260-B1EE-A6A0A4CAADC3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>